<commit_message>
Intermediate Commit to switch device
</commit_message>
<xml_diff>
--- a/evaluation/assets/generated_files/prediction_df.xlsx
+++ b/evaluation/assets/generated_files/prediction_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:G1"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,856 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>c8:4e:8c:fb:78:f8</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1559376000000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>319.1588855410767</v>
+      </c>
+      <c r="F2" t="n">
+        <v>34.51077386469305</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1271.289938322596</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>16:0a:79:df:2f:af</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1559376000000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>123.55593834195</v>
+      </c>
+      <c r="F3" t="n">
+        <v>201.0872359949732</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1133.624222127414</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9a:7d:ba:09:5b:6d</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1559376000000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>160.8346932189537</v>
+      </c>
+      <c r="F4" t="n">
+        <v>237.8412029441139</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1111.720485168001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>57:d4:a8:d1:58:2f</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1559376000000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>208.4207052536922</v>
+      </c>
+      <c r="F5" t="n">
+        <v>163.5852132030133</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1112.973126479226</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>19:c8:c0:61:68:36</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1559376000000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>123.7190524172525</v>
+      </c>
+      <c r="F6" t="n">
+        <v>201.1769990668278</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1132.057358373127</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>16:0a:79:df:2f:af</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1559376001000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>122.9390042128433</v>
+      </c>
+      <c r="F7" t="n">
+        <v>201.0065299520433</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1131.294817718091</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>9a:7d:ba:09:5b:6d</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1559376001000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>159.7373842718717</v>
+      </c>
+      <c r="F8" t="n">
+        <v>238.2424226695177</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1091.165227115862</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>c8:4e:8c:fb:78:f8</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1559376001000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>319.9118544539928</v>
+      </c>
+      <c r="F9" t="n">
+        <v>34.98743494905487</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1264.62697926163</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>19:c8:c0:61:68:36</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1559376001000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>123.7310055859478</v>
+      </c>
+      <c r="F10" t="n">
+        <v>201.6783462842127</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1124.785779052298</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>9a:7d:ba:09:5b:6d</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1559376002000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>158.0989836441144</v>
+      </c>
+      <c r="F11" t="n">
+        <v>239.2489068893584</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1065.773172964938</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>c8:4e:8c:fb:78:f8</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1559376002000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>319.9771468015537</v>
+      </c>
+      <c r="F12" t="n">
+        <v>35.96840030895337</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1256.688434215425</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19:c8:c0:61:68:36</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1559376002000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>123.7446926782318</v>
+      </c>
+      <c r="F13" t="n">
+        <v>202.3754750081026</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1114.630633684456</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>16:0a:79:df:2f:af</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1559376002000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>123.1931570489738</v>
+      </c>
+      <c r="F14" t="n">
+        <v>201.5469775739552</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1113.898907790939</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>19:c8:c0:61:68:36</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1559376003000</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>123.7500100318033</v>
+      </c>
+      <c r="F15" t="n">
+        <v>203.2081746364137</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1102.335415599393</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>c8:4e:8c:fb:78:f8</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1559376003000</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>320.0382226959202</v>
+      </c>
+      <c r="F16" t="n">
+        <v>37.30374138946827</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1248.506665687758</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:0a:79:df:2f:af</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1559376003000</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>123.3315545769108</v>
+      </c>
+      <c r="F17" t="n">
+        <v>203.3484277727976</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1085.176123962141</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>9a:7d:ba:09:5b:6d</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1559376003000</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>156.249981010295</v>
+      </c>
+      <c r="F18" t="n">
+        <v>240.6100779088564</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1040.047746466506</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>9a:7d:ba:09:5b:6d</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1559376004000</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>154.4815344522984</v>
+      </c>
+      <c r="F19" t="n">
+        <v>242.2646074936596</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1020.030043704208</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>19:c8:c0:61:68:36</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1559376004000</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>123.7368539843612</v>
+      </c>
+      <c r="F20" t="n">
+        <v>204.1162345670624</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1088.643618126902</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>16:0a:79:df:2f:af</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1559376004000</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>123.8053662757111</v>
+      </c>
+      <c r="F21" t="n">
+        <v>206.3915296112041</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1044.122592448922</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>c8:4e:8c:fb:78:f8</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1559376004000</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>320.7551735471699</v>
+      </c>
+      <c r="F22" t="n">
+        <v>39.19887356843331</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1240.934069474927</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>19:c8:c0:61:68:36</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1559376005000</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>123.6951208736043</v>
+      </c>
+      <c r="F23" t="n">
+        <v>205.039444197965</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1074.298734596774</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>c8:4e:8c:fb:78:f8</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1559376005000</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>321.070980251094</v>
+      </c>
+      <c r="F24" t="n">
+        <v>39.77431717384452</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1239.75322353705</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>16:0a:79:df:2f:af</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1559376005000</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>123.6904684122559</v>
+      </c>
+      <c r="F25" t="n">
+        <v>207.5335416283505</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1033.167897412951</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>14:97:8b:87:46:68</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1559376005000</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>321.4414284027639</v>
+      </c>
+      <c r="F26" t="n">
+        <v>38.4716328352588</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1257.620657209697</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>c8:4e:8c:fb:78:f8</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1559376006000</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>320.9792474372781</v>
+      </c>
+      <c r="F27" t="n">
+        <v>39.90966980312358</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1236.994015779471</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>19:c8:c0:61:68:36</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>1559376006000</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="n">
+        <v>123.6147070372313</v>
+      </c>
+      <c r="F28" t="n">
+        <v>205.9175929270376</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1060.044258338804</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>16:0a:79:df:2f:af</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1559376006000</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" t="n">
+        <v>123.3922103911303</v>
+      </c>
+      <c r="F29" t="n">
+        <v>207.8218589382587</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1033.040743685442</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>19:c8:c0:61:68:36</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1559376007000</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" t="n">
+        <v>123.4855088129411</v>
+      </c>
+      <c r="F30" t="n">
+        <v>206.6904701521966</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1046.623682682784</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>c8:4e:8c:fb:78:f8</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1559376007000</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>320.4070927786457</v>
+      </c>
+      <c r="F31" t="n">
+        <v>40.0444965512721</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1235.528737812027</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>16:0a:79:df:2f:af</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1559376007000</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>123.0174992922134</v>
+      </c>
+      <c r="F32" t="n">
+        <v>207.4812657559084</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1038.389704080985</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>16:0a:79:df:2f:af</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>1559376008000</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>122.8680260552245</v>
+      </c>
+      <c r="F33" t="n">
+        <v>206.69101418634</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1040.205945409481</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>19:c8:c0:61:68:36</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1559376008000</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" t="n">
+        <v>123.2263794952908</v>
+      </c>
+      <c r="F34" t="n">
+        <v>207.2036048691492</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1035.117438538698</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>c8:4e:8c:fb:78:f8</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>1559376008000</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="n">
+        <v>320.244190524238</v>
+      </c>
+      <c r="F35" t="n">
+        <v>40.12498676541709</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1234.639942636542</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>